<commit_message>
UC on Steel scrap share
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_IIS.xlsx
+++ b/suppxls/Scen_UC_IIS.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F952D-1C5C-4A83-B36A-71BC54057751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E925954-DE0C-47F6-8D67-798342C7B447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9345" yWindow="8475" windowWidth="21840" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4110" yWindow="-18615" windowWidth="31245" windowHeight="16935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel Scrap ratio" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>UC_N</t>
   </si>
@@ -550,10 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:X36"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -567,10 +568,10 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="37.85546875" customWidth="1"/>
+    <col min="18" max="18" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -587,7 +588,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:20">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>14</v>
@@ -604,7 +605,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:20">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>10</v>
@@ -621,7 +622,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:20">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -638,7 +639,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:20">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>0</v>
@@ -677,74 +678,60 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:20">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" t="str">
-        <f>R36</f>
-        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISSCREAF-E,IISBFBOF-N,IISDRIEAF-NG,IISSCREAF-N,IISHDRIEAF-N</v>
-      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
+      <c r="K6" s="1"/>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:20">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" t="str">
-        <f>R17</f>
-        <v>IISSCREAF-E,IISSCREAF-N</v>
-      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>2017</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
+      <c r="K7" s="1"/>
       <c r="L7" s="1">
-        <v>-0.3</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="2" t="str">
-        <f>D7</f>
+      <c r="D8" t="str">
+        <f>R18</f>
         <v>IISSCREAF-E,IISSCREAF-N</v>
       </c>
       <c r="E8" s="1"/>
@@ -752,28 +739,22 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <v>2030</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1"/>
       <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>-0.3</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="2" t="str">
+      <c r="D9" t="str">
         <f>D8</f>
         <v>IISSCREAF-E,IISSCREAF-N</v>
       </c>
@@ -782,99 +763,193 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1">
+        <v>2017</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1">
+        <f>1+K13</f>
+        <v>0.7</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2" t="str">
+        <f>D8</f>
+        <v>IISSCREAF-E,IISSCREAF-N</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>2030</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K11" si="0">1+K14</f>
+        <v>0.7</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2" t="str">
+        <f>D10</f>
+        <v>IISSCREAF-E,IISSCREAF-N</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
         <v>2050</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="str">
+        <f>R35</f>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N,IISDRIEAF-NG,IISHDRIEAF-N</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="str">
+        <f>D12</f>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N,IISDRIEAF-NG,IISHDRIEAF-N</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2017</v>
+      </c>
+      <c r="K13" s="1">
         <v>-0.3</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
-      <c r="T15" s="9" t="s">
+    </row>
+    <row r="14" spans="1:20">
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="str">
+        <f>D13</f>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N,IISDRIEAF-NG,IISHDRIEAF-N</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2030</v>
+      </c>
+      <c r="K14" s="1">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="str">
+        <f>D14</f>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N,IISDRIEAF-NG,IISHDRIEAF-N</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2050</v>
+      </c>
+      <c r="K15" s="1">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="T16" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
-      <c r="R16" s="2" t="str">
-        <f>T16</f>
+    <row r="17" spans="18:24">
+      <c r="R17" s="2" t="str">
+        <f>T17</f>
         <v>IISSCREAF-E</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T17" t="s">
         <v>16</v>
       </c>
-      <c r="X16" s="2"/>
-    </row>
-    <row r="17" spans="18:20">
-      <c r="R17" s="2" t="str">
-        <f>R16&amp;","&amp;T17</f>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="18:24">
+      <c r="R18" s="2" t="str">
+        <f>R17&amp;","&amp;T18</f>
         <v>IISSCREAF-E,IISSCREAF-N</v>
       </c>
-      <c r="T17" s="8" t="s">
+      <c r="T18" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="18:20">
-      <c r="T27" s="9" t="s">
+    <row r="28" spans="18:24">
+      <c r="T28" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="18:20">
-      <c r="R28" s="2" t="str">
-        <f>T28</f>
+    <row r="29" spans="18:24">
+      <c r="R29" s="2" t="str">
+        <f>T29</f>
         <v>IISBFBOF-E</v>
       </c>
-      <c r="T28" t="s">
+      <c r="T29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="18:20">
-      <c r="R29" s="2" t="str">
-        <f>R28&amp;","&amp;T29</f>
+    <row r="30" spans="18:24">
+      <c r="R30" s="2" t="str">
+        <f>R29&amp;","&amp;T30</f>
         <v>IISBFBOF-E,IISDRIEAF-E</v>
       </c>
-      <c r="T29" t="s">
+      <c r="T30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="18:20">
-      <c r="R30" s="2" t="str">
-        <f t="shared" ref="R30:R36" si="0">R29&amp;","&amp;T30</f>
+    <row r="31" spans="18:24">
+      <c r="R31" s="2" t="str">
+        <f t="shared" ref="R31:R37" si="1">R30&amp;","&amp;T31</f>
         <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E</v>
       </c>
-      <c r="T30" t="s">
+      <c r="T31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="18:20">
-      <c r="R31" s="2" t="str">
-        <f t="shared" si="0"/>
+    <row r="32" spans="18:24">
+      <c r="R32" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E</v>
       </c>
-      <c r="T31" t="s">
+      <c r="T32" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="18:20">
-      <c r="R32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISSCREAF-E</v>
-      </c>
-      <c r="T32" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="33" spans="18:20">
       <c r="R33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISSCREAF-E,IISBFBOF-N</v>
+        <f t="shared" si="1"/>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N</v>
       </c>
       <c r="T33" t="s">
         <v>23</v>
@@ -882,8 +957,8 @@
     </row>
     <row r="34" spans="18:20">
       <c r="R34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISSCREAF-E,IISBFBOF-N,IISDRIEAF-NG</v>
+        <f t="shared" si="1"/>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N,IISDRIEAF-NG</v>
       </c>
       <c r="T34" t="s">
         <v>24</v>
@@ -891,21 +966,19 @@
     </row>
     <row r="35" spans="18:20">
       <c r="R35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISSCREAF-E,IISBFBOF-N,IISDRIEAF-NG,IISSCREAF-N</v>
-      </c>
-      <c r="T35" s="8" t="s">
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISBFBOF-N,IISDRIEAF-NG,IISHDRIEAF-N</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="18:20">
-      <c r="R36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>IISBFBOF-E,IISDRIEAF-E,IISCOREAF-E,IISOTHEAF-E,IISSCREAF-E,IISBFBOF-N,IISDRIEAF-NG,IISSCREAF-N,IISHDRIEAF-N</v>
-      </c>
-      <c r="T36" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="R36" s="2"/>
+      <c r="T36" s="8"/>
+    </row>
+    <row r="37" spans="18:20">
+      <c r="R37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>